<commit_message>
prototype ready unit conversions cm to mm still missing
</commit_message>
<xml_diff>
--- a/Work hours.xlsx
+++ b/Work hours.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AtteR\PycharmProjects\maler1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E1F7347-BFD3-468B-BA49-6EDC3D2641F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95152BF3-AB7E-4B7A-A68D-5A7005DB8D37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="840" yWindow="-120" windowWidth="37680" windowHeight="21840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6150" yWindow="3270" windowWidth="31125" windowHeight="17100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -47,7 +47,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="d\.m\.yyyy;@"/>
+    <numFmt numFmtId="164" formatCode="d\.m\.yyyy;@"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -91,8 +91,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normaali" xfId="0" builtinId="0"/>
@@ -376,7 +376,7 @@
   <dimension ref="A1:C52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -412,7 +412,7 @@
         <v>44479</v>
       </c>
       <c r="B3" s="2">
-        <v>6.5</v>
+        <v>9</v>
       </c>
       <c r="C3" t="s">
         <v>3</v>

</xml_diff>